<commit_message>
Ethylene consumed to almost zero
</commit_message>
<xml_diff>
--- a/pp_gas_enrichments/NM2_2_DifferentialCentrifugation1.xlsx
+++ b/pp_gas_enrichments/NM2_2_DifferentialCentrifugation1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH4" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{03D0B9DC-61AA-4364-A10B-08571DA09EDF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+calibration average 0.5%ch4=1909.45</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -60,13 +94,16 @@
   </si>
   <si>
     <t>18kg_1.5hour_8</t>
+  </si>
+  <si>
+    <t>dif</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +126,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -118,6 +168,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,11 +453,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:AL9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,56 +466,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="10"/>
+      <c r="K2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7" t="s">
+      <c r="L2" s="10"/>
+      <c r="M2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7" t="s">
+      <c r="N2" s="10"/>
+      <c r="O2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7" t="s">
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7" t="s">
+      <c r="R2" s="10"/>
+      <c r="S2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AL2" s="7"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
     </row>
     <row r="3" spans="3:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -633,68 +686,124 @@
         <v>1281.98</v>
       </c>
     </row>
-    <row r="6" spans="3:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="3">
+    <row r="6" spans="3:38" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5">
         <v>42979</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="6">
         <f>C6-C4</f>
         <v>9</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <v>477</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="6">
         <v>1240.6500000000001</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="6">
         <v>491.9</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="6">
         <v>1279.43</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="6">
         <v>490.91</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="6">
         <v>1278.8</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="6">
         <v>483.22899999999998</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="6">
         <v>1256.8489999999999</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="6">
         <v>501.87</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="6">
         <v>1305.3699999999999</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="6">
         <v>471.99</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="6">
         <v>1227.5899999999999</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="6">
         <v>476.99</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="6">
         <v>1240</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="6">
         <v>489.5</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6" s="6">
         <v>1273.26</v>
       </c>
     </row>
-    <row r="7" spans="3:38" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
+    <row r="7" spans="3:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>42986</v>
+      </c>
+      <c r="D7" s="1">
+        <f>C7-C4</f>
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <v>466.7</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1220.9000000000001</v>
+      </c>
+      <c r="G7" s="1">
+        <v>477.14</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1248.26</v>
+      </c>
+      <c r="I7" s="1">
+        <v>474.63</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1241.67</v>
+      </c>
+      <c r="K7" s="1">
+        <v>467.67</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1223.45</v>
+      </c>
+      <c r="M7" s="1">
+        <v>490.39</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1282.95</v>
+      </c>
+      <c r="O7" s="1">
+        <v>454.94</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1190.0999999999999</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>469.45</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1212.28</v>
+      </c>
+      <c r="S7" s="1">
+        <v>479.74</v>
+      </c>
+      <c r="T7" s="1">
+        <v>1255</v>
+      </c>
     </row>
     <row r="8" spans="3:38" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="3:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
@@ -721,6 +830,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -728,76 +838,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:AP8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="10"/>
+      <c r="K2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7" t="s">
+      <c r="L2" s="10"/>
+      <c r="M2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7" t="s">
+      <c r="N2" s="10"/>
+      <c r="O2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7" t="s">
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7" t="s">
+      <c r="R2" s="10"/>
+      <c r="S2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AL2" s="7"/>
-      <c r="AM2" s="7"/>
-      <c r="AN2" s="7"/>
-      <c r="AO2" s="7"/>
-      <c r="AP2" s="7"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="10"/>
+      <c r="AP2" s="10"/>
     </row>
     <row r="3" spans="3:42" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -853,7 +964,7 @@
       <c r="C4" s="2">
         <v>42970</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <v>0</v>
       </c>
       <c r="AM4" s="4"/>
@@ -865,7 +976,7 @@
       <c r="C5" s="5">
         <v>42975</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="9">
         <f>C5-C4</f>
         <v>5</v>
       </c>
@@ -918,65 +1029,119 @@
         <v>9.1899999999999996E-2</v>
       </c>
     </row>
-    <row r="6" spans="3:42" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="3">
+    <row r="6" spans="3:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5">
         <v>42979</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="9">
         <f>C6-C4</f>
         <v>9</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <v>37</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="6">
         <v>0.1114</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="6">
         <v>36.770000000000003</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="6">
         <v>0.1106</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="6">
         <v>24.5</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="6">
         <v>7.3800000000000004E-2</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="6">
         <v>25.7</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="6">
         <v>7.7399999999999997E-2</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="6">
         <v>21.53</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="6">
         <v>6.4799999999999996E-2</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="6">
         <v>24.25</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="6">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="6">
         <v>20.399999999999999</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="6">
         <v>6.1400000000000003E-2</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="6">
         <v>19.12</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6" s="6">
         <v>5.7500000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="3:42" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="3"/>
+      <c r="C7" s="3">
+        <v>42986</v>
+      </c>
+      <c r="D7" s="8">
+        <f>C7-C4</f>
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45.28</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.13769999999999999</v>
+      </c>
+      <c r="G7" s="1">
+        <v>41.68</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.1268</v>
+      </c>
+      <c r="I7" s="1">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="K7" s="1">
+        <v>24.3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M7" s="1">
+        <v>23.859000000000002</v>
+      </c>
+      <c r="N7" s="1">
+        <v>7.2599999999999998E-2</v>
+      </c>
+      <c r="O7" s="1">
+        <v>24.68</v>
+      </c>
+      <c r="P7" s="1">
+        <v>7.51E-2</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="R7" s="1">
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="S7" s="1">
+        <v>21.89</v>
+      </c>
+      <c r="T7" s="1">
+        <v>6.7000000000000004E-2</v>
+      </c>
     </row>
     <row r="8" spans="3:42" x14ac:dyDescent="0.25">
       <c r="AE8" s="1"/>

</xml_diff>

<commit_message>
EthyleneCH4mix_Ethylene_CH4 on diff centr
</commit_message>
<xml_diff>
--- a/pp_gas_enrichments/NM2_2_DifferentialCentrifugation1.xlsx
+++ b/pp_gas_enrichments/NM2_2_DifferentialCentrifugation1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -50,12 +50,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{3666E4DB-A05B-4822-ADB8-102B21A236DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+refilling ch4 with 0.75 ml of 'pure ch4' in the samples 1-3</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -96,14 +120,48 @@
     <t>18kg_1.5hour_8</t>
   </si>
   <si>
-    <t>dif</t>
+    <t>stdCh4</t>
+  </si>
+  <si>
+    <t>StdCO2</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,17 +185,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,20 +220,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="18" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,379 +525,668 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:AL9"/>
+  <dimension ref="A2:AM13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="15"/>
+    <col min="3" max="3" width="10.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="15" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="E2" s="10" t="s">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="16"/>
+      <c r="H2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="16"/>
+      <c r="L2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="16"/>
+      <c r="N2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="16"/>
+      <c r="P2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="16"/>
+      <c r="T2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-    </row>
-    <row r="3" spans="3:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="16"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="16"/>
+      <c r="AK2" s="16"/>
+      <c r="AL2" s="16"/>
+      <c r="AM2" s="16"/>
+    </row>
+    <row r="3" spans="1:39" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" s="17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C4" s="2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C4" s="18">
         <v>42970</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="19">
+        <v>0.55972222222222201</v>
+      </c>
+      <c r="E4" s="15">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="F4" s="15">
         <v>474.38</v>
       </c>
-      <c r="F4">
+      <c r="G4" s="15">
         <v>1233</v>
       </c>
-      <c r="G4">
+      <c r="H4" s="15">
         <v>490.25</v>
       </c>
-      <c r="H4">
+      <c r="I4" s="15">
         <v>1274.71</v>
       </c>
-      <c r="I4">
+      <c r="J4" s="15">
         <v>488.2</v>
       </c>
-      <c r="J4">
+      <c r="K4" s="15">
         <v>1269.5</v>
       </c>
-      <c r="K4">
+      <c r="L4" s="15">
         <v>488.5</v>
       </c>
-      <c r="L4">
+      <c r="M4" s="15">
         <v>1270</v>
       </c>
-      <c r="M4">
+      <c r="N4" s="15">
         <v>508.9</v>
       </c>
-      <c r="N4">
+      <c r="O4" s="15">
         <v>1323.2</v>
       </c>
-      <c r="O4">
+      <c r="P4" s="15">
         <v>473.85</v>
       </c>
-      <c r="P4">
+      <c r="Q4" s="15">
         <v>1232</v>
       </c>
-      <c r="Q4">
+      <c r="R4" s="15">
         <v>493.16</v>
       </c>
-      <c r="R4">
+      <c r="S4" s="15">
         <v>1282</v>
       </c>
-      <c r="S4">
+      <c r="T4" s="15">
         <v>493.57</v>
       </c>
-      <c r="T4">
+      <c r="U4" s="15">
         <v>1283</v>
       </c>
     </row>
-    <row r="5" spans="3:38" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="5">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C5" s="18">
         <v>42975</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="19">
+        <v>0.55972222222222201</v>
+      </c>
+      <c r="E5" s="15">
         <f>C5-C4</f>
         <v>5</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="15">
         <v>466.89</v>
       </c>
-      <c r="F5" s="6">
+      <c r="G5" s="15">
         <v>1241.3900000000001</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="15">
         <v>486.95</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="15">
         <v>1294.8</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="15">
         <v>479.7</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="15">
         <v>1275.5</v>
       </c>
-      <c r="K5" s="6">
+      <c r="L5" s="15">
         <v>459.47</v>
       </c>
-      <c r="L5" s="6">
+      <c r="M5" s="15">
         <v>1221.6500000000001</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="15">
         <v>496.38</v>
       </c>
-      <c r="N5" s="6">
+      <c r="O5" s="15">
         <v>1319.89</v>
       </c>
-      <c r="O5" s="6">
+      <c r="P5" s="15">
         <v>462.53</v>
       </c>
-      <c r="P5" s="6">
+      <c r="Q5" s="15">
         <v>1229.78</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="R5" s="15">
         <v>472.35</v>
       </c>
-      <c r="R5" s="6">
+      <c r="S5" s="15">
         <v>1255</v>
       </c>
-      <c r="S5" s="6">
+      <c r="T5" s="15">
         <v>482.12</v>
       </c>
-      <c r="T5" s="6">
+      <c r="U5" s="15">
         <v>1281.98</v>
       </c>
     </row>
-    <row r="6" spans="3:38" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="5">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C6" s="18">
         <v>42979</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="19">
+        <v>0.55972222222222201</v>
+      </c>
+      <c r="E6" s="15">
         <f>C6-C4</f>
         <v>9</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="15">
         <v>477</v>
       </c>
-      <c r="F6" s="6">
+      <c r="G6" s="15">
         <v>1240.6500000000001</v>
       </c>
-      <c r="G6" s="6">
+      <c r="H6" s="15">
         <v>491.9</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="15">
         <v>1279.43</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="15">
         <v>490.91</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="15">
         <v>1278.8</v>
       </c>
-      <c r="K6" s="6">
+      <c r="L6" s="15">
         <v>483.22899999999998</v>
       </c>
-      <c r="L6" s="6">
+      <c r="M6" s="15">
         <v>1256.8489999999999</v>
       </c>
-      <c r="M6" s="6">
+      <c r="N6" s="15">
         <v>501.87</v>
       </c>
-      <c r="N6" s="6">
+      <c r="O6" s="15">
         <v>1305.3699999999999</v>
       </c>
-      <c r="O6" s="6">
+      <c r="P6" s="15">
         <v>471.99</v>
       </c>
-      <c r="P6" s="6">
+      <c r="Q6" s="15">
         <v>1227.5899999999999</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="R6" s="15">
         <v>476.99</v>
       </c>
-      <c r="R6" s="6">
+      <c r="S6" s="15">
         <v>1240</v>
       </c>
-      <c r="S6" s="6">
+      <c r="T6" s="15">
         <v>489.5</v>
       </c>
-      <c r="T6" s="6">
+      <c r="U6" s="15">
         <v>1273.26</v>
       </c>
     </row>
-    <row r="7" spans="3:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="3">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C7" s="18">
         <v>42986</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="19">
+        <v>0.55972222222222201</v>
+      </c>
+      <c r="E7" s="15">
         <f>C7-C4</f>
         <v>16</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="15">
         <v>466.7</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="15">
         <v>1220.9000000000001</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="15">
         <v>477.14</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="15">
         <v>1248.26</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="15">
         <v>474.63</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="15">
         <v>1241.67</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="15">
         <v>467.67</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="15">
         <v>1223.45</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="15">
         <v>490.39</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="15">
         <v>1282.95</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="15">
         <v>454.94</v>
       </c>
-      <c r="P7" s="1">
+      <c r="Q7" s="15">
         <v>1190.0999999999999</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="R7" s="15">
         <v>469.45</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="15">
         <v>1212.28</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="15">
         <v>479.74</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U7" s="15">
         <v>1255</v>
       </c>
     </row>
-    <row r="8" spans="3:38" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="3:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>5000</v>
+      </c>
+      <c r="B8" s="15">
+        <v>1899.9</v>
+      </c>
+      <c r="C8" s="18">
+        <v>43004</v>
+      </c>
+      <c r="D8" s="19">
+        <v>0.55972222222222201</v>
+      </c>
+      <c r="E8" s="15">
+        <f>C8-$C$4</f>
+        <v>34</v>
+      </c>
+      <c r="F8" s="15">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="G8" s="15">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="H8" s="15">
+        <v>33.49</v>
+      </c>
+      <c r="I8" s="15">
+        <v>88.05</v>
+      </c>
+      <c r="J8" s="15">
+        <v>3.99</v>
+      </c>
+      <c r="K8" s="15">
+        <v>7.415</v>
+      </c>
+      <c r="L8" s="15">
+        <v>258.87</v>
+      </c>
+      <c r="M8" s="15">
+        <v>678.55</v>
+      </c>
+      <c r="N8" s="15">
+        <v>496.54</v>
+      </c>
+      <c r="O8" s="15">
+        <v>1304.3900000000001</v>
+      </c>
+      <c r="P8" s="15">
+        <v>466.47</v>
+      </c>
+      <c r="Q8" s="15">
+        <v>1225.21</v>
+      </c>
+      <c r="R8" s="15">
+        <v>484.46</v>
+      </c>
+      <c r="S8" s="15">
+        <v>1272.58</v>
+      </c>
+      <c r="T8" s="15">
+        <v>565.25</v>
+      </c>
+      <c r="U8" s="15">
+        <v>1485.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>5000</v>
+      </c>
+      <c r="B9" s="15">
+        <v>1941</v>
+      </c>
+      <c r="C9" s="18">
+        <v>43004</v>
+      </c>
+      <c r="D9" s="19">
+        <v>0.55972222222222201</v>
+      </c>
+      <c r="E9" s="15">
+        <f>C9-$C$4</f>
+        <v>34</v>
+      </c>
+      <c r="F9" s="15">
+        <v>84.29</v>
+      </c>
+      <c r="G9" s="15">
+        <v>214.66</v>
+      </c>
+      <c r="H9" s="15">
+        <v>113.7</v>
+      </c>
+      <c r="I9" s="15">
+        <v>290.5</v>
+      </c>
+      <c r="J9" s="15">
+        <v>101.02</v>
+      </c>
+      <c r="K9" s="15">
+        <v>257.77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>5000</v>
+      </c>
+      <c r="B10" s="15">
+        <v>1928</v>
+      </c>
+      <c r="C10" s="18">
+        <v>43006</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.55972222222222223</v>
+      </c>
+      <c r="E10" s="15">
+        <f>C10-$C$4</f>
+        <v>36</v>
+      </c>
+      <c r="F10" s="15">
+        <v>31.24</v>
+      </c>
+      <c r="G10" s="15">
+        <v>78.37</v>
+      </c>
+      <c r="H10" s="15">
+        <v>42.6</v>
+      </c>
+      <c r="I10" s="15">
+        <v>107.89</v>
+      </c>
+      <c r="J10" s="15">
+        <v>39.21</v>
+      </c>
+      <c r="K10" s="15">
+        <v>99</v>
+      </c>
+      <c r="L10" s="15">
+        <v>91.2</v>
+      </c>
+      <c r="M10" s="15">
+        <v>234.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>5000</v>
+      </c>
+      <c r="B11" s="15">
+        <v>1861.9</v>
+      </c>
+      <c r="C11" s="18">
+        <v>43007</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.55972222222222223</v>
+      </c>
+      <c r="E11" s="15">
+        <f>C11-$C$4</f>
+        <v>37</v>
+      </c>
+      <c r="F11" s="15">
+        <v>14.4</v>
+      </c>
+      <c r="G11" s="15">
+        <v>35.119999999999997</v>
+      </c>
+      <c r="H11" s="15">
+        <v>21.8</v>
+      </c>
+      <c r="I11" s="15">
+        <v>54.89</v>
+      </c>
+      <c r="J11" s="15">
+        <v>14.53</v>
+      </c>
+      <c r="K11" s="15">
+        <v>35.35</v>
+      </c>
+      <c r="L11" s="15">
+        <v>38.18</v>
+      </c>
+      <c r="M11" s="15">
+        <v>98.91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>5000</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1866</v>
+      </c>
+      <c r="C12" s="3">
+        <v>43008</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.35138888888888892</v>
+      </c>
+      <c r="E12" s="4">
+        <f>C12-$C$4</f>
+        <v>38</v>
+      </c>
+      <c r="F12" s="4">
+        <v>9.14</v>
+      </c>
+      <c r="G12" s="4">
+        <v>20.97</v>
+      </c>
+      <c r="H12" s="4">
+        <v>14.84</v>
+      </c>
+      <c r="I12" s="4">
+        <v>36.18</v>
+      </c>
+      <c r="J12" s="4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="K12" s="4">
+        <v>19.77</v>
+      </c>
+      <c r="L12" s="4">
+        <v>19.66</v>
+      </c>
+      <c r="M12" s="4">
+        <v>49.09</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1936</v>
+      </c>
+      <c r="C13" s="2">
+        <v>43011</v>
+      </c>
+      <c r="D13" s="13">
+        <v>0.66527777777777775</v>
+      </c>
+      <c r="E13" s="1">
+        <f>C13-$C$4</f>
+        <v>41</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="G13" s="1">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4.12</v>
+      </c>
+      <c r="I13" s="1">
+        <v>8</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2.42</v>
+      </c>
+      <c r="L13" s="1">
+        <v>3</v>
+      </c>
+      <c r="M13" s="1">
+        <v>5.2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -836,147 +1196,158 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C2:AP8"/>
+  <dimension ref="A2:AP11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="6"/>
+    <col min="3" max="3" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="E2" s="10" t="s">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="E2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10" t="s">
+      <c r="N2" s="14"/>
+      <c r="O2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10" t="s">
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10" t="s">
+      <c r="R2" s="14"/>
+      <c r="S2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10"/>
-    </row>
-    <row r="3" spans="3:42" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="14"/>
+    </row>
+    <row r="3" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="K3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="M3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="1" t="s">
+      <c r="O3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="1" t="s">
+      <c r="Q3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T3" s="1" t="s">
+      <c r="S3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="C4" s="2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="C4" s="10">
         <v>42970</v>
       </c>
       <c r="D4" s="7">
         <v>0</v>
       </c>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-    </row>
-    <row r="5" spans="3:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="5">
+      <c r="AM4" s="11"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="11"/>
+      <c r="AP4" s="11"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="C5" s="10">
         <v>42975</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <f>C5-C4</f>
         <v>5</v>
       </c>
@@ -1029,11 +1400,11 @@
         <v>9.1899999999999996E-2</v>
       </c>
     </row>
-    <row r="6" spans="3:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="5">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="C6" s="10">
         <v>42979</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <f>C6-C4</f>
         <v>9</v>
       </c>
@@ -1086,66 +1457,200 @@
         <v>5.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="3:42" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="3">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="C7" s="10">
         <v>42986</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <f>C7-C4</f>
         <v>16</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <v>45.28</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="6">
         <v>0.13769999999999999</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="6">
         <v>41.68</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="6">
         <v>0.1268</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="6">
         <v>33.299999999999997</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="6">
         <v>0.10100000000000001</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="6">
         <v>24.3</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="6">
         <v>23.859000000000002</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="6">
         <v>7.2599999999999998E-2</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="6">
         <v>24.68</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="6">
         <v>7.51E-2</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7" s="6">
         <v>22.5</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="6">
         <v>6.8500000000000005E-2</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="6">
         <v>21.89</v>
       </c>
-      <c r="T7" s="1">
+      <c r="T7" s="6">
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="8" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6">
+        <v>314.65899999999999</v>
+      </c>
+      <c r="C8" s="10">
+        <v>43004</v>
+      </c>
+      <c r="D8" s="7">
+        <f>C8-$C$4</f>
+        <v>34</v>
+      </c>
+      <c r="E8" s="6">
+        <v>86.07</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.27360000000000001</v>
+      </c>
+      <c r="G8" s="6">
+        <v>67.03</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="I8" s="6">
+        <v>49.37</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.156</v>
+      </c>
+      <c r="K8" s="6">
+        <v>33.69</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0.107</v>
+      </c>
+      <c r="M8" s="6">
+        <v>22.68</v>
+      </c>
+      <c r="N8" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O8" s="6">
+        <v>25.24</v>
+      </c>
+      <c r="P8" s="6">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>20.440000000000001</v>
+      </c>
+      <c r="R8" s="6">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="S8" s="6">
+        <v>20.79</v>
+      </c>
+      <c r="T8" s="6">
+        <v>6.6100000000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="C9" s="10">
+        <v>43006</v>
+      </c>
+      <c r="D9" s="7">
+        <f>C9-$C$4</f>
+        <v>36</v>
+      </c>
+      <c r="E9" s="6">
+        <v>87.85</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G9" s="6">
+        <v>74</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.249</v>
+      </c>
+      <c r="I9" s="6">
+        <v>58.4</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.19</v>
+      </c>
+      <c r="K9" s="6">
+        <v>42.79</v>
+      </c>
+      <c r="L9" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4">
+        <v>312.60000000000002</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43007</v>
+      </c>
+      <c r="D10" s="5">
+        <f>C10-$C$4</f>
+        <v>37</v>
+      </c>
+      <c r="E10" s="4">
+        <v>84.2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="G10" s="4">
+        <v>72.459999999999994</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.23180000000000001</v>
+      </c>
+      <c r="I10" s="4">
+        <v>49.59</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="K10" s="4">
+        <v>46.48</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0.14799999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="C11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>